<commit_message>
Add images for new cards: 000-190
</commit_message>
<xml_diff>
--- a/card-design/cards.xlsx
+++ b/card-design/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoey\git\open-card-game\card-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA380B2-1656-4DA2-B967-8822EFF6D3D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F60934F-12EA-45A1-94CB-0B48A5B91D0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="144" windowWidth="31920" windowHeight="24516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="408" windowWidth="31920" windowHeight="24516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="1" r:id="rId1"/>
@@ -970,9 +970,6 @@
     <t>Your spells cost [Any] less.</t>
   </si>
   <si>
-    <t>Lian, Master Sorcerer</t>
-  </si>
-  <si>
     <t>Spirit Sprite</t>
   </si>
   <si>
@@ -1111,9 +1108,6 @@
     <t>Wish</t>
   </si>
   <si>
-    <t>Banish all creatures. Both players discard their hands. Draw 3 cards.</t>
-  </si>
-  <si>
     <t>Prophet Valeriya</t>
   </si>
   <si>
@@ -1262,6 +1256,12 @@
   </si>
   <si>
     <t>Summon a 1 / 1 [Fire] Fire Worshipper token.</t>
+  </si>
+  <si>
+    <t>Exile all creatures. Both players discard their hands. Draw 3 cards.</t>
+  </si>
+  <si>
+    <t>Lian, Gem Of The South</t>
   </si>
 </sst>
 </file>
@@ -1792,259 +1792,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF9C0006"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b val="0"/>
@@ -2114,8 +1862,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>112392</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Element">
@@ -2138,7 +1886,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2192,8 +1940,8 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>180973</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Type">
@@ -2216,7 +1964,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2293,9 +2041,9 @@
   <sortState ref="A2:I192">
     <sortCondition ref="C2:C192" customList="Earth,Fire,Water,Air,Spirit"/>
     <sortCondition ref="D2:D192" customList="Hero,Creature,Spell,Item"/>
-    <sortCondition sortBy="fontColor" ref="F2:F192" dxfId="3"/>
+    <sortCondition sortBy="fontColor" ref="F2:F192" dxfId="1"/>
     <sortCondition ref="F2:F192"/>
-    <sortCondition sortBy="fontColor" ref="E2:E192" dxfId="2"/>
+    <sortCondition sortBy="fontColor" ref="E2:E192" dxfId="0"/>
     <sortCondition ref="E2:E192" customList="Reaction,Enchantment,Equipment,Permanent,Field"/>
     <sortCondition ref="B2:B192"/>
   </sortState>
@@ -2613,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2701,7 +2449,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -2716,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2963,7 +2711,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -2972,7 +2720,7 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2981,7 +2729,7 @@
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2989,7 +2737,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -3015,7 +2763,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -3024,7 +2772,7 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -3377,7 +3125,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -3386,10 +3134,10 @@
         <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I33" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -3397,7 +3145,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C34" t="s">
         <v>10</v>
@@ -3406,10 +3154,10 @@
         <v>15</v>
       </c>
       <c r="F34" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I34" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -3779,7 +3527,7 @@
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -3813,7 +3561,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C53" t="s">
         <v>69</v>
@@ -3831,7 +3579,7 @@
         <v>3</v>
       </c>
       <c r="I53" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -4215,7 +3963,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C71" t="s">
         <v>69</v>
@@ -4230,7 +3978,7 @@
         <v>77</v>
       </c>
       <c r="I71" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -4238,7 +3986,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C72" t="s">
         <v>69</v>
@@ -4253,7 +4001,7 @@
         <v>77</v>
       </c>
       <c r="I72" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -4284,7 +4032,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C74" t="s">
         <v>69</v>
@@ -4293,10 +4041,10 @@
         <v>15</v>
       </c>
       <c r="F74" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I74" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -4553,7 +4301,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C87" t="s">
         <v>69</v>
@@ -4568,7 +4316,7 @@
         <v>265</v>
       </c>
       <c r="I87" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -4728,7 +4476,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C95" t="s">
         <v>123</v>
@@ -4737,7 +4485,7 @@
         <v>11</v>
       </c>
       <c r="F95" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G95">
         <v>3</v>
@@ -5044,7 +4792,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C109" t="s">
         <v>123</v>
@@ -5053,10 +4801,10 @@
         <v>15</v>
       </c>
       <c r="F109" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I109" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
@@ -5064,7 +4812,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C110" t="s">
         <v>123</v>
@@ -5076,10 +4824,10 @@
         <v>16</v>
       </c>
       <c r="F110" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I110" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
@@ -5087,7 +4835,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C111" t="s">
         <v>123</v>
@@ -5099,7 +4847,7 @@
         <v>142</v>
       </c>
       <c r="I111" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
@@ -5517,7 +5265,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>311</v>
+        <v>408</v>
       </c>
       <c r="C131" t="s">
         <v>249</v>
@@ -5698,7 +5446,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C139" t="s">
         <v>249</v>
@@ -5707,7 +5455,7 @@
         <v>11</v>
       </c>
       <c r="F139" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G139">
         <v>3</v>
@@ -5716,7 +5464,7 @@
         <v>4</v>
       </c>
       <c r="I139" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
@@ -6077,7 +5825,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C156" t="s">
         <v>249</v>
@@ -6092,7 +5840,7 @@
         <v>17</v>
       </c>
       <c r="I156" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
@@ -6100,7 +5848,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C157" t="s">
         <v>249</v>
@@ -6112,10 +5860,10 @@
         <v>16</v>
       </c>
       <c r="F157" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I157" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
@@ -6186,7 +5934,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C161" t="s">
         <v>249</v>
@@ -6198,10 +5946,10 @@
         <v>47</v>
       </c>
       <c r="F161" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I161" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
@@ -6300,19 +6048,19 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C167" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D167" t="s">
         <v>44</v>
       </c>
       <c r="F167" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I167" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
@@ -6320,10 +6068,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C168" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D168" t="s">
         <v>11</v>
@@ -6340,10 +6088,10 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C169" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D169" t="s">
         <v>11</v>
@@ -6355,7 +6103,7 @@
         <v>1</v>
       </c>
       <c r="I169" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
@@ -6363,10 +6111,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
+        <v>311</v>
+      </c>
+      <c r="C170" t="s">
         <v>312</v>
-      </c>
-      <c r="C170" t="s">
-        <v>313</v>
       </c>
       <c r="D170" t="s">
         <v>11</v>
@@ -6378,7 +6126,7 @@
         <v>1</v>
       </c>
       <c r="I170" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
@@ -6386,16 +6134,16 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C171" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D171" t="s">
         <v>11</v>
       </c>
       <c r="F171" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G171">
         <v>2</v>
@@ -6404,7 +6152,7 @@
         <v>2</v>
       </c>
       <c r="I171" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
@@ -6412,16 +6160,16 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C172" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D172" t="s">
         <v>11</v>
       </c>
       <c r="F172" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G172">
         <v>1</v>
@@ -6430,7 +6178,7 @@
         <v>2</v>
       </c>
       <c r="I172" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
@@ -6438,16 +6186,16 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C173" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D173" t="s">
         <v>11</v>
       </c>
       <c r="F173" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G173">
         <v>2</v>
@@ -6456,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="I173" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
@@ -6464,16 +6212,16 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C174" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
       </c>
       <c r="F174" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G174">
         <v>3</v>
@@ -6482,7 +6230,7 @@
         <v>3</v>
       </c>
       <c r="I174" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
@@ -6490,16 +6238,16 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C175" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D175" t="s">
         <v>11</v>
       </c>
       <c r="F175" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G175">
         <v>4</v>
@@ -6508,7 +6256,7 @@
         <v>4</v>
       </c>
       <c r="I175" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
@@ -6516,16 +6264,16 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
+        <v>344</v>
+      </c>
+      <c r="C176" t="s">
+        <v>312</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+      <c r="I176" t="s">
         <v>345</v>
-      </c>
-      <c r="C176" t="s">
-        <v>313</v>
-      </c>
-      <c r="D176" t="s">
-        <v>15</v>
-      </c>
-      <c r="I176" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
@@ -6533,16 +6281,16 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
+        <v>328</v>
+      </c>
+      <c r="C177" t="s">
+        <v>312</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+      <c r="I177" t="s">
         <v>329</v>
-      </c>
-      <c r="C177" t="s">
-        <v>313</v>
-      </c>
-      <c r="D177" t="s">
-        <v>15</v>
-      </c>
-      <c r="I177" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
@@ -6550,16 +6298,16 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
+        <v>332</v>
+      </c>
+      <c r="C178" t="s">
+        <v>312</v>
+      </c>
+      <c r="D178" t="s">
+        <v>15</v>
+      </c>
+      <c r="I178" t="s">
         <v>333</v>
-      </c>
-      <c r="C178" t="s">
-        <v>313</v>
-      </c>
-      <c r="D178" t="s">
-        <v>15</v>
-      </c>
-      <c r="I178" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
@@ -6567,16 +6315,16 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
+        <v>330</v>
+      </c>
+      <c r="C179" t="s">
+        <v>312</v>
+      </c>
+      <c r="D179" t="s">
+        <v>15</v>
+      </c>
+      <c r="I179" t="s">
         <v>331</v>
-      </c>
-      <c r="C179" t="s">
-        <v>313</v>
-      </c>
-      <c r="D179" t="s">
-        <v>15</v>
-      </c>
-      <c r="I179" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
@@ -6584,19 +6332,19 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
+        <v>388</v>
+      </c>
+      <c r="C180" t="s">
+        <v>312</v>
+      </c>
+      <c r="D180" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" t="s">
+        <v>389</v>
+      </c>
+      <c r="I180" t="s">
         <v>390</v>
-      </c>
-      <c r="C180" t="s">
-        <v>313</v>
-      </c>
-      <c r="D180" t="s">
-        <v>15</v>
-      </c>
-      <c r="F180" t="s">
-        <v>391</v>
-      </c>
-      <c r="I180" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
@@ -6604,19 +6352,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
+        <v>338</v>
+      </c>
+      <c r="C181" t="s">
+        <v>312</v>
+      </c>
+      <c r="D181" t="s">
+        <v>15</v>
+      </c>
+      <c r="F181" t="s">
+        <v>314</v>
+      </c>
+      <c r="I181" t="s">
         <v>339</v>
-      </c>
-      <c r="C181" t="s">
-        <v>313</v>
-      </c>
-      <c r="D181" t="s">
-        <v>15</v>
-      </c>
-      <c r="F181" t="s">
-        <v>315</v>
-      </c>
-      <c r="I181" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
@@ -6624,19 +6372,19 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
+        <v>350</v>
+      </c>
+      <c r="C182" t="s">
+        <v>312</v>
+      </c>
+      <c r="D182" t="s">
+        <v>15</v>
+      </c>
+      <c r="F182" t="s">
+        <v>314</v>
+      </c>
+      <c r="I182" t="s">
         <v>351</v>
-      </c>
-      <c r="C182" t="s">
-        <v>313</v>
-      </c>
-      <c r="D182" t="s">
-        <v>15</v>
-      </c>
-      <c r="F182" t="s">
-        <v>315</v>
-      </c>
-      <c r="I182" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
@@ -6644,19 +6392,19 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
+        <v>334</v>
+      </c>
+      <c r="C183" t="s">
+        <v>312</v>
+      </c>
+      <c r="D183" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" t="s">
+        <v>314</v>
+      </c>
+      <c r="I183" t="s">
         <v>335</v>
-      </c>
-      <c r="C183" t="s">
-        <v>313</v>
-      </c>
-      <c r="D183" t="s">
-        <v>15</v>
-      </c>
-      <c r="F183" t="s">
-        <v>315</v>
-      </c>
-      <c r="I183" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
@@ -6664,10 +6412,10 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C184" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D184" t="s">
         <v>15</v>
@@ -6676,10 +6424,10 @@
         <v>16</v>
       </c>
       <c r="F184" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I184" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
@@ -6687,10 +6435,10 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C185" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D185" t="s">
         <v>15</v>
@@ -6699,10 +6447,10 @@
         <v>20</v>
       </c>
       <c r="F185" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I185" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
@@ -6710,10 +6458,10 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C186" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D186" t="s">
         <v>15</v>
@@ -6722,10 +6470,10 @@
         <v>47</v>
       </c>
       <c r="F186" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I186" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
@@ -6733,10 +6481,10 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C187" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D187" t="s">
         <v>15</v>
@@ -6745,7 +6493,7 @@
         <v>16</v>
       </c>
       <c r="F187" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I187" t="s">
         <v>225</v>
@@ -6756,10 +6504,10 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C188" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D188" t="s">
         <v>15</v>
@@ -6768,10 +6516,10 @@
         <v>47</v>
       </c>
       <c r="F188" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I188" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
@@ -6779,10 +6527,10 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C189" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D189" t="s">
         <v>15</v>
@@ -6791,10 +6539,10 @@
         <v>20</v>
       </c>
       <c r="F189" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I189" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
@@ -6802,19 +6550,19 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
+        <v>353</v>
+      </c>
+      <c r="C190" t="s">
+        <v>312</v>
+      </c>
+      <c r="D190" t="s">
+        <v>15</v>
+      </c>
+      <c r="F190" t="s">
         <v>354</v>
       </c>
-      <c r="C190" t="s">
-        <v>313</v>
-      </c>
-      <c r="D190" t="s">
-        <v>15</v>
-      </c>
-      <c r="F190" t="s">
+      <c r="I190" t="s">
         <v>355</v>
-      </c>
-      <c r="I190" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
@@ -6822,19 +6570,19 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C191" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D191" t="s">
         <v>15</v>
       </c>
       <c r="F191" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I191" t="s">
-        <v>358</v>
+        <v>407</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
@@ -6842,10 +6590,10 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C192" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D192" t="s">
         <v>27</v>
@@ -6854,15 +6602,15 @@
         <v>41</v>
       </c>
       <c r="F192" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I192" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>$J$1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add Real cost element
</commit_message>
<xml_diff>
--- a/card-design/cards.xlsx
+++ b/card-design/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoey\git\open-card-game\card-design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F60934F-12EA-45A1-94CB-0B48A5B91D0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70555675-080D-4E51-A72B-CF5357B6D42A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="408" windowWidth="31920" windowHeight="24516" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="6216" windowWidth="27312" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cards" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="412">
   <si>
     <t>ID</t>
   </si>
@@ -1262,6 +1262,15 @@
   </si>
   <si>
     <t>Lian, Gem Of The South</t>
+  </si>
+  <si>
+    <t>Human Man</t>
+  </si>
+  <si>
+    <t>1e,1r</t>
+  </si>
+  <si>
+    <t>Oioi.</t>
   </si>
 </sst>
 </file>
@@ -1852,18 +1861,18 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>6811108</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>22857</xdr:rowOff>
+      <xdr:colOff>4947139</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>69749</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>8639908</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>112392</xdr:rowOff>
+      <xdr:colOff>6775939</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>117232</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Element">
@@ -1886,7 +1895,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1896,8 +1905,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12954000" y="931395"/>
-              <a:ext cx="1828800" cy="2451735"/>
+              <a:off x="10884877" y="3885611"/>
+              <a:ext cx="1828800" cy="1682852"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1930,18 +1939,18 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>6750733</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>91438</xdr:rowOff>
+      <xdr:colOff>4957103</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>56269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>8579533</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>180973</xdr:rowOff>
+      <xdr:colOff>6785903</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>17584</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-      <mc:Choice Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Type">
@@ -1964,7 +1973,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1974,8 +1983,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="12893625" y="3543884"/>
-              <a:ext cx="1828800" cy="2451735"/>
+              <a:off x="10894841" y="2418469"/>
+              <a:ext cx="1828800" cy="1414977"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2036,8 +2045,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I192" totalsRowShown="0">
-  <autoFilter ref="A1:I192" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I193" totalsRowShown="0">
+  <autoFilter ref="A1:I193" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A2:I192">
     <sortCondition ref="C2:C192" customList="Earth,Fire,Water,Air,Spirit"/>
     <sortCondition ref="D2:D192" customList="Hero,Creature,Spell,Item"/>
@@ -2359,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I192"/>
+  <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B168" sqref="B168"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2372,6 +2381,9 @@
     <col min="3" max="3" width="9.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" customWidth="1"/>
     <col min="9" max="9" width="140.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6606,6 +6618,32 @@
       </c>
       <c r="I192" t="s">
         <v>360</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>191</v>
+      </c>
+      <c r="B193" t="s">
+        <v>409</v>
+      </c>
+      <c r="C193" t="s">
+        <v>10</v>
+      </c>
+      <c r="D193" t="s">
+        <v>11</v>
+      </c>
+      <c r="F193" t="s">
+        <v>410</v>
+      </c>
+      <c r="G193">
+        <v>2</v>
+      </c>
+      <c r="H193">
+        <v>2</v>
+      </c>
+      <c r="I193" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>